<commit_message>
working on lecture 1
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="922">
   <si>
     <t xml:space="preserve">survived</t>
   </si>
@@ -2780,18 +2780,12 @@
   </si>
   <si>
     <t xml:space="preserve">carb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -3110,10 +3104,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -26212,10 +26206,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -41731,10 +41725,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -41795,11 +41789,11 @@
       <c r="G2" t="n">
         <v>16.46</v>
       </c>
-      <c r="H2" t="s">
-        <v>922</v>
-      </c>
-      <c r="I2" t="s">
-        <v>923</v>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
       </c>
       <c r="J2" t="n">
         <v>4</v>
@@ -41830,11 +41824,11 @@
       <c r="G3" t="n">
         <v>17.02</v>
       </c>
-      <c r="H3" t="s">
-        <v>922</v>
-      </c>
-      <c r="I3" t="s">
-        <v>923</v>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
       </c>
       <c r="J3" t="n">
         <v>4</v>
@@ -41865,11 +41859,11 @@
       <c r="G4" t="n">
         <v>18.61</v>
       </c>
-      <c r="H4" t="s">
-        <v>923</v>
-      </c>
-      <c r="I4" t="s">
-        <v>923</v>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
       </c>
       <c r="J4" t="n">
         <v>4</v>
@@ -41900,11 +41894,11 @@
       <c r="G5" t="n">
         <v>19.44</v>
       </c>
-      <c r="H5" t="s">
-        <v>923</v>
-      </c>
-      <c r="I5" t="s">
-        <v>922</v>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
       </c>
       <c r="J5" t="n">
         <v>3</v>
@@ -41935,11 +41929,11 @@
       <c r="G6" t="n">
         <v>17.02</v>
       </c>
-      <c r="H6" t="s">
-        <v>922</v>
-      </c>
-      <c r="I6" t="s">
-        <v>922</v>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>3</v>
@@ -41970,11 +41964,11 @@
       <c r="G7" t="n">
         <v>20.22</v>
       </c>
-      <c r="H7" t="s">
-        <v>923</v>
-      </c>
-      <c r="I7" t="s">
-        <v>922</v>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
       </c>
       <c r="J7" t="n">
         <v>3</v>
@@ -42005,11 +41999,11 @@
       <c r="G8" t="n">
         <v>15.84</v>
       </c>
-      <c r="H8" t="s">
-        <v>922</v>
-      </c>
-      <c r="I8" t="s">
-        <v>922</v>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
       </c>
       <c r="J8" t="n">
         <v>3</v>
@@ -42040,11 +42034,11 @@
       <c r="G9" t="n">
         <v>20</v>
       </c>
-      <c r="H9" t="s">
-        <v>923</v>
-      </c>
-      <c r="I9" t="s">
-        <v>922</v>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
       </c>
       <c r="J9" t="n">
         <v>4</v>
@@ -42075,11 +42069,11 @@
       <c r="G10" t="n">
         <v>22.9</v>
       </c>
-      <c r="H10" t="s">
-        <v>923</v>
-      </c>
-      <c r="I10" t="s">
-        <v>922</v>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
       </c>
       <c r="J10" t="n">
         <v>4</v>
@@ -42110,11 +42104,11 @@
       <c r="G11" t="n">
         <v>18.3</v>
       </c>
-      <c r="H11" t="s">
-        <v>923</v>
-      </c>
-      <c r="I11" t="s">
-        <v>922</v>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
       </c>
       <c r="J11" t="n">
         <v>4</v>
@@ -42145,11 +42139,11 @@
       <c r="G12" t="n">
         <v>18.9</v>
       </c>
-      <c r="H12" t="s">
-        <v>923</v>
-      </c>
-      <c r="I12" t="s">
-        <v>922</v>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
       </c>
       <c r="J12" t="n">
         <v>4</v>
@@ -42180,11 +42174,11 @@
       <c r="G13" t="n">
         <v>17.4</v>
       </c>
-      <c r="H13" t="s">
-        <v>922</v>
-      </c>
-      <c r="I13" t="s">
-        <v>922</v>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
       </c>
       <c r="J13" t="n">
         <v>3</v>
@@ -42215,11 +42209,11 @@
       <c r="G14" t="n">
         <v>17.6</v>
       </c>
-      <c r="H14" t="s">
-        <v>922</v>
-      </c>
-      <c r="I14" t="s">
-        <v>922</v>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
       </c>
       <c r="J14" t="n">
         <v>3</v>
@@ -42250,11 +42244,11 @@
       <c r="G15" t="n">
         <v>18</v>
       </c>
-      <c r="H15" t="s">
-        <v>922</v>
-      </c>
-      <c r="I15" t="s">
-        <v>922</v>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
       </c>
       <c r="J15" t="n">
         <v>3</v>
@@ -42285,11 +42279,11 @@
       <c r="G16" t="n">
         <v>17.98</v>
       </c>
-      <c r="H16" t="s">
-        <v>922</v>
-      </c>
-      <c r="I16" t="s">
-        <v>922</v>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
       </c>
       <c r="J16" t="n">
         <v>3</v>
@@ -42320,11 +42314,11 @@
       <c r="G17" t="n">
         <v>17.82</v>
       </c>
-      <c r="H17" t="s">
-        <v>922</v>
-      </c>
-      <c r="I17" t="s">
-        <v>922</v>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
       </c>
       <c r="J17" t="n">
         <v>3</v>
@@ -42355,11 +42349,11 @@
       <c r="G18" t="n">
         <v>17.42</v>
       </c>
-      <c r="H18" t="s">
-        <v>922</v>
-      </c>
-      <c r="I18" t="s">
-        <v>922</v>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
       </c>
       <c r="J18" t="n">
         <v>3</v>
@@ -42390,11 +42384,11 @@
       <c r="G19" t="n">
         <v>19.47</v>
       </c>
-      <c r="H19" t="s">
-        <v>923</v>
-      </c>
-      <c r="I19" t="s">
-        <v>923</v>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
       </c>
       <c r="J19" t="n">
         <v>4</v>
@@ -42425,11 +42419,11 @@
       <c r="G20" t="n">
         <v>18.52</v>
       </c>
-      <c r="H20" t="s">
-        <v>923</v>
-      </c>
-      <c r="I20" t="s">
-        <v>923</v>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
       </c>
       <c r="J20" t="n">
         <v>4</v>
@@ -42460,11 +42454,11 @@
       <c r="G21" t="n">
         <v>19.9</v>
       </c>
-      <c r="H21" t="s">
-        <v>923</v>
-      </c>
-      <c r="I21" t="s">
-        <v>923</v>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
       </c>
       <c r="J21" t="n">
         <v>4</v>
@@ -42495,11 +42489,11 @@
       <c r="G22" t="n">
         <v>20.01</v>
       </c>
-      <c r="H22" t="s">
-        <v>923</v>
-      </c>
-      <c r="I22" t="s">
-        <v>922</v>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
       </c>
       <c r="J22" t="n">
         <v>3</v>
@@ -42530,11 +42524,11 @@
       <c r="G23" t="n">
         <v>16.87</v>
       </c>
-      <c r="H23" t="s">
-        <v>922</v>
-      </c>
-      <c r="I23" t="s">
-        <v>922</v>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
       </c>
       <c r="J23" t="n">
         <v>3</v>
@@ -42565,11 +42559,11 @@
       <c r="G24" t="n">
         <v>17.3</v>
       </c>
-      <c r="H24" t="s">
-        <v>922</v>
-      </c>
-      <c r="I24" t="s">
-        <v>922</v>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
       </c>
       <c r="J24" t="n">
         <v>3</v>
@@ -42600,11 +42594,11 @@
       <c r="G25" t="n">
         <v>15.41</v>
       </c>
-      <c r="H25" t="s">
-        <v>922</v>
-      </c>
-      <c r="I25" t="s">
-        <v>922</v>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
       </c>
       <c r="J25" t="n">
         <v>3</v>
@@ -42635,11 +42629,11 @@
       <c r="G26" t="n">
         <v>17.05</v>
       </c>
-      <c r="H26" t="s">
-        <v>922</v>
-      </c>
-      <c r="I26" t="s">
-        <v>922</v>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
       </c>
       <c r="J26" t="n">
         <v>3</v>
@@ -42670,11 +42664,11 @@
       <c r="G27" t="n">
         <v>18.9</v>
       </c>
-      <c r="H27" t="s">
-        <v>923</v>
-      </c>
-      <c r="I27" t="s">
-        <v>923</v>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1</v>
       </c>
       <c r="J27" t="n">
         <v>4</v>
@@ -42705,11 +42699,11 @@
       <c r="G28" t="n">
         <v>16.7</v>
       </c>
-      <c r="H28" t="s">
-        <v>922</v>
-      </c>
-      <c r="I28" t="s">
-        <v>923</v>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1</v>
       </c>
       <c r="J28" t="n">
         <v>5</v>
@@ -42740,11 +42734,11 @@
       <c r="G29" t="n">
         <v>16.9</v>
       </c>
-      <c r="H29" t="s">
-        <v>923</v>
-      </c>
-      <c r="I29" t="s">
-        <v>923</v>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1</v>
       </c>
       <c r="J29" t="n">
         <v>5</v>
@@ -42775,11 +42769,11 @@
       <c r="G30" t="n">
         <v>14.5</v>
       </c>
-      <c r="H30" t="s">
-        <v>922</v>
-      </c>
-      <c r="I30" t="s">
-        <v>923</v>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
       </c>
       <c r="J30" t="n">
         <v>5</v>
@@ -42810,11 +42804,11 @@
       <c r="G31" t="n">
         <v>15.5</v>
       </c>
-      <c r="H31" t="s">
-        <v>922</v>
-      </c>
-      <c r="I31" t="s">
-        <v>923</v>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
       </c>
       <c r="J31" t="n">
         <v>5</v>
@@ -42845,11 +42839,11 @@
       <c r="G32" t="n">
         <v>14.6</v>
       </c>
-      <c r="H32" t="s">
-        <v>922</v>
-      </c>
-      <c r="I32" t="s">
-        <v>923</v>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
       </c>
       <c r="J32" t="n">
         <v>5</v>
@@ -42880,11 +42874,11 @@
       <c r="G33" t="n">
         <v>18.6</v>
       </c>
-      <c r="H33" t="s">
-        <v>923</v>
-      </c>
-      <c r="I33" t="s">
-        <v>923</v>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
       </c>
       <c r="J33" t="n">
         <v>4</v>

</xml_diff>